<commit_message>
dangtq them mau 3b
</commit_message>
<xml_diff>
--- a/Business/Application_Of_Trademark.xlsx
+++ b/Business/Application_Of_Trademark.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7403AF07-370C-43F7-8564-4CD045E3F8B3}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9525" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>Request for amendment of application</t>
   </si>
@@ -247,11 +248,20 @@
   <si>
     <t>Link Data by Application</t>
   </si>
+  <si>
+    <t>Trạng thái</t>
+  </si>
+  <si>
+    <t>Đã chốt</t>
+  </si>
+  <si>
+    <t>Đang trao đổi</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -328,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -348,9 +358,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -627,23 +643,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
-    <col min="4" max="4" width="50.42578125" customWidth="1"/>
-    <col min="5" max="5" width="39.7109375" customWidth="1"/>
-    <col min="6" max="6" width="55.28515625" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" customWidth="1"/>
+    <col min="6" max="6" width="39.7109375" customWidth="1"/>
+    <col min="7" max="7" width="55.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -651,263 +668,287 @@
         <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="7"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>34</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="6" t="s">
+      <c r="C3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>36</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="2" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>37</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="2" t="s">
+      <c r="C6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="2" t="s">
+      <c r="C7" s="7"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="2" t="s">
+      <c r="C8" s="7"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="7"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>42</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="7"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="2" t="s">
+      <c r="C11" s="7"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="7"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>46</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="2" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="2" t="s">
+      <c r="C14" s="7"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>49</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="3"/>
-      <c r="D15" s="2" t="s">
+      <c r="C15" s="7"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="2" t="s">
+      <c r="C16" s="7"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>